<commit_message>
add apple to sample_porfiolio
</commit_message>
<xml_diff>
--- a/sample_portfolio.xlsx
+++ b/sample_portfolio.xlsx
@@ -493,17 +493,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -513,17 +513,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10.07.2025 23:29</t>
+          <t>14.09.2025 17:24</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>7.4375</v>
+        <v>5.5397</v>
       </c>
       <c r="G2" t="n">
-        <v>122.62</v>
+        <v>56.67</v>
       </c>
       <c r="H2" t="n">
-        <v>911.99</v>
+        <v>313.93</v>
       </c>
       <c r="I2" t="n">
         <v>1</v>
@@ -536,17 +536,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -556,17 +556,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09.07.2025 11:23</t>
+          <t>16.08.2025 02:20</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3.5822</v>
+        <v>6.5058</v>
       </c>
       <c r="G3" t="n">
-        <v>100</v>
+        <v>25.56</v>
       </c>
       <c r="H3" t="n">
-        <v>358.22</v>
+        <v>166.29</v>
       </c>
       <c r="I3" t="n">
         <v>1</v>
@@ -574,155 +574,151 @@
       <c r="J3" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="n">
-        <v>0.91</v>
-      </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>14.09.2025 13:46</t>
+          <t>13.08.2025 02:11</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>4.3953</v>
+        <v>9.3378</v>
       </c>
       <c r="G4" t="n">
-        <v>57.7</v>
+        <v>74.3</v>
       </c>
       <c r="H4" t="n">
-        <v>253.61</v>
+        <v>693.8</v>
       </c>
       <c r="I4" t="n">
-        <v>2.3719</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>-6.11</v>
+        <v>0</v>
       </c>
       <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09.10.2025 00:30</t>
+          <t>31.08.2025 19:21</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>2.8557</v>
+        <v>9.0626</v>
       </c>
       <c r="G5" t="n">
-        <v>76.05</v>
+        <v>183.53</v>
       </c>
       <c r="H5" t="n">
-        <v>217.18</v>
+        <v>1663.26</v>
       </c>
       <c r="I5" t="n">
-        <v>1</v>
+        <v>2.9405</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>-2.23</v>
       </c>
       <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>11.10.2025 10:55</t>
+          <t>26.09.2025 18:53</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>2.6681</v>
+        <v>7.0292</v>
       </c>
       <c r="G6" t="n">
-        <v>100</v>
+        <v>189.59</v>
       </c>
       <c r="H6" t="n">
-        <v>266.81</v>
+        <v>1332.67</v>
       </c>
       <c r="I6" t="n">
-        <v>1</v>
+        <v>2.8522</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>8.84</v>
-      </c>
+        <v>-7.52</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -732,17 +728,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>19.07.2025 08:36</t>
+          <t>02.09.2025 16:09</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>1.898</v>
+        <v>6.8746</v>
       </c>
       <c r="G7" t="n">
-        <v>100</v>
+        <v>29.62</v>
       </c>
       <c r="H7" t="n">
-        <v>189.8</v>
+        <v>203.63</v>
       </c>
       <c r="I7" t="n">
         <v>1</v>
@@ -750,14 +746,12 @@
       <c r="J7" t="n">
         <v>0</v>
       </c>
-      <c r="K7" t="n">
-        <v>5.85</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -777,17 +771,17 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>03.07.2025 19:05</t>
+          <t>04.08.2025 13:14</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>5.8797</v>
+        <v>8.672599999999999</v>
       </c>
       <c r="G8" t="n">
         <v>100</v>
       </c>
       <c r="H8" t="n">
-        <v>587.97</v>
+        <v>867.26</v>
       </c>
       <c r="I8" t="n">
         <v>1</v>
@@ -796,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0.87</v>
+        <v>7.52</v>
       </c>
     </row>
     <row r="9">
@@ -822,17 +816,17 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>10.07.2025 21:08</t>
+          <t>13.10.2025 10:42</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0.8098</v>
+        <v>3.7099</v>
       </c>
       <c r="G9" t="n">
-        <v>183.6</v>
+        <v>56.62</v>
       </c>
       <c r="H9" t="n">
-        <v>148.68</v>
+        <v>210.05</v>
       </c>
       <c r="I9" t="n">
         <v>1</v>
@@ -845,17 +839,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -865,40 +859,40 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>14.10.2025 04:01</t>
+          <t>29.07.2025 13:23</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5.2194</v>
+        <v>9.8446</v>
       </c>
       <c r="G10" t="n">
-        <v>60.55</v>
+        <v>78.90000000000001</v>
       </c>
       <c r="H10" t="n">
-        <v>316.03</v>
+        <v>776.74</v>
       </c>
       <c r="I10" t="n">
-        <v>3.55</v>
+        <v>1.9415</v>
       </c>
       <c r="J10" t="n">
-        <v>-2.33</v>
+        <v>1.7</v>
       </c>
       <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -908,17 +902,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>29.07.2025 00:31</t>
+          <t>14.08.2025 00:35</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>9.1921</v>
+        <v>2.718</v>
       </c>
       <c r="G11" t="n">
-        <v>100</v>
+        <v>172.39</v>
       </c>
       <c r="H11" t="n">
-        <v>919.21</v>
+        <v>468.56</v>
       </c>
       <c r="I11" t="n">
         <v>1</v>
@@ -926,67 +920,67 @@
       <c r="J11" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="n">
-        <v>7.06</v>
-      </c>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>19.08.2025 15:45</t>
+          <t>02.10.2025 19:48</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>8.6526</v>
+        <v>8.2478</v>
       </c>
       <c r="G12" t="n">
-        <v>56.23</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>486.54</v>
+        <v>824.78</v>
       </c>
       <c r="I12" t="n">
-        <v>1.2744</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.77</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>7.19</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -996,17 +990,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>03.07.2025 23:32</t>
+          <t>24.10.2025 02:14</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>8.857799999999999</v>
+        <v>0.7877999999999999</v>
       </c>
       <c r="G13" t="n">
-        <v>100</v>
+        <v>88.03</v>
       </c>
       <c r="H13" t="n">
-        <v>885.78</v>
+        <v>69.34999999999999</v>
       </c>
       <c r="I13" t="n">
         <v>1</v>
@@ -1014,19 +1008,17 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
-      <c r="K13" t="n">
-        <v>3.35</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1036,45 +1028,45 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>20.10.2025 09:03</t>
+          <t>02.08.2025 17:56</t>
         </is>
       </c>
       <c r="F14" t="n">
-        <v>1.8985</v>
+        <v>5.0585</v>
       </c>
       <c r="G14" t="n">
-        <v>142.2</v>
+        <v>197.56</v>
       </c>
       <c r="H14" t="n">
-        <v>269.97</v>
+        <v>999.36</v>
       </c>
       <c r="I14" t="n">
-        <v>3.1553</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>-2.9</v>
+        <v>0</v>
       </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1084,17 +1076,17 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>08.09.2025 23:47</t>
+          <t>01.09.2025 02:50</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>4.6525</v>
+        <v>3.7531</v>
       </c>
       <c r="G15" t="n">
-        <v>100</v>
+        <v>76.76000000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>465.25</v>
+        <v>288.09</v>
       </c>
       <c r="I15" t="n">
         <v>1</v>
@@ -1102,19 +1094,17 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
-      <c r="K15" t="n">
-        <v>2.57</v>
-      </c>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1124,45 +1114,45 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>03.07.2025 15:00</t>
+          <t>06.07.2025 16:15</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>9.0853</v>
+        <v>6.3576</v>
       </c>
       <c r="G16" t="n">
-        <v>135.11</v>
+        <v>51.79</v>
       </c>
       <c r="H16" t="n">
-        <v>1227.51</v>
+        <v>329.26</v>
       </c>
       <c r="I16" t="n">
-        <v>1</v>
+        <v>2.7244</v>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>-5.56</v>
       </c>
       <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1172,17 +1162,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>27.09.2025 18:16</t>
+          <t>27.08.2025 00:35</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>8.5128</v>
+        <v>7.7888</v>
       </c>
       <c r="G17" t="n">
-        <v>100</v>
+        <v>17.55</v>
       </c>
       <c r="H17" t="n">
-        <v>851.28</v>
+        <v>136.69</v>
       </c>
       <c r="I17" t="n">
         <v>1</v>
@@ -1190,9 +1180,7 @@
       <c r="J17" t="n">
         <v>0</v>
       </c>
-      <c r="K17" t="n">
-        <v>7.91</v>
-      </c>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1217,17 +1205,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>11.07.2025 23:05</t>
+          <t>11.07.2025 08:01</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>8.677899999999999</v>
+        <v>8.388299999999999</v>
       </c>
       <c r="G18" t="n">
         <v>100</v>
       </c>
       <c r="H18" t="n">
-        <v>867.79</v>
+        <v>838.83</v>
       </c>
       <c r="I18" t="n">
         <v>1</v>
@@ -1236,18 +1224,18 @@
         <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>5.3</v>
+        <v>9.960000000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1262,17 +1250,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>13.10.2025 08:00</t>
+          <t>05.09.2025 20:09</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>9.5472</v>
+        <v>6.035</v>
       </c>
       <c r="G19" t="n">
         <v>100</v>
       </c>
       <c r="H19" t="n">
-        <v>954.72</v>
+        <v>603.5</v>
       </c>
       <c r="I19" t="n">
         <v>1</v>
@@ -1281,23 +1269,23 @@
         <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>1.21</v>
+        <v>6.38</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1307,17 +1295,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>27.08.2025 16:31</t>
+          <t>29.10.2025 09:04</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>1.1469</v>
+        <v>3.5168</v>
       </c>
       <c r="G20" t="n">
-        <v>87.06999999999999</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>99.86</v>
+        <v>351.68</v>
       </c>
       <c r="I20" t="n">
         <v>1</v>
@@ -1325,62 +1313,62 @@
       <c r="J20" t="n">
         <v>0</v>
       </c>
-      <c r="K20" t="inlineStr"/>
+      <c r="K20" t="n">
+        <v>2.59</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>02.07.2025 07:05</t>
+          <t>21.08.2025 05:55</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>0.7817</v>
+        <v>4.4101</v>
       </c>
       <c r="G21" t="n">
-        <v>100</v>
+        <v>199.88</v>
       </c>
       <c r="H21" t="n">
-        <v>78.17</v>
+        <v>881.49</v>
       </c>
       <c r="I21" t="n">
-        <v>1</v>
+        <v>3.6769</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>7.89</v>
-      </c>
+        <v>-5.02</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1395,17 +1383,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>23.07.2025 20:17</t>
+          <t>08.08.2025 06:58</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.7462</v>
+        <v>5.2821</v>
       </c>
       <c r="G22" t="n">
         <v>100</v>
       </c>
       <c r="H22" t="n">
-        <v>74.62</v>
+        <v>528.21</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -1414,56 +1402,58 @@
         <v>0</v>
       </c>
       <c r="K22" t="n">
-        <v>6.91</v>
+        <v>8.52</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>01.08.2025 06:31</t>
+          <t>05.09.2025 11:35</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>8.247299999999999</v>
+        <v>5.1604</v>
       </c>
       <c r="G23" t="n">
-        <v>84.26000000000001</v>
+        <v>100</v>
       </c>
       <c r="H23" t="n">
-        <v>694.92</v>
+        <v>516.04</v>
       </c>
       <c r="I23" t="n">
-        <v>3.7306</v>
+        <v>1</v>
       </c>
       <c r="J23" t="n">
-        <v>-8.98</v>
-      </c>
-      <c r="K23" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>8.029999999999999</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1483,17 +1473,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>13.10.2025 17:17</t>
+          <t>29.09.2025 07:11</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>-0.0975</v>
+        <v>-0.1608</v>
       </c>
       <c r="G24" t="n">
         <v>100</v>
       </c>
       <c r="H24" t="n">
-        <v>-9.75</v>
+        <v>-16.08</v>
       </c>
       <c r="I24" t="n">
         <v>1</v>
@@ -1502,23 +1492,23 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>9.17</v>
+        <v>5.64</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1528,17 +1518,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>09.07.2025 10:42</t>
+          <t>30.07.2025 06:02</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>1.3634</v>
+        <v>7.5593</v>
       </c>
       <c r="G25" t="n">
-        <v>163.25</v>
+        <v>100</v>
       </c>
       <c r="H25" t="n">
-        <v>222.58</v>
+        <v>755.9299999999999</v>
       </c>
       <c r="I25" t="n">
         <v>1</v>
@@ -1546,7 +1536,9 @@
       <c r="J25" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="n">
+        <v>2.49</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1571,17 +1563,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>23.10.2025 14:44</t>
+          <t>12.09.2025 18:28</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>2.402</v>
+        <v>4.691</v>
       </c>
       <c r="G26" t="n">
         <v>100</v>
       </c>
       <c r="H26" t="n">
-        <v>240.2</v>
+        <v>469.1</v>
       </c>
       <c r="I26" t="n">
         <v>1</v>
@@ -1590,23 +1582,23 @@
         <v>0</v>
       </c>
       <c r="K26" t="n">
-        <v>2.82</v>
+        <v>1.38</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1616,17 +1608,17 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>27.10.2025 19:44</t>
+          <t>20.08.2025 22:04</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>1.9201</v>
+        <v>0.4192</v>
       </c>
       <c r="G27" t="n">
-        <v>80.43000000000001</v>
+        <v>100</v>
       </c>
       <c r="H27" t="n">
-        <v>154.43</v>
+        <v>41.92</v>
       </c>
       <c r="I27" t="n">
         <v>1</v>
@@ -1634,7 +1626,9 @@
       <c r="J27" t="n">
         <v>0</v>
       </c>
-      <c r="K27" t="inlineStr"/>
+      <c r="K27" t="n">
+        <v>9.890000000000001</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1659,30 +1653,30 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>02.10.2025 01:25</t>
+          <t>07.09.2025 14:25</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>4.0756</v>
+        <v>6.4497</v>
       </c>
       <c r="G28" t="n">
-        <v>68.92</v>
+        <v>79.45999999999999</v>
       </c>
       <c r="H28" t="n">
-        <v>280.89</v>
+        <v>512.49</v>
       </c>
       <c r="I28" t="n">
-        <v>3.6956</v>
+        <v>1.4988</v>
       </c>
       <c r="J28" t="n">
-        <v>-8.25</v>
+        <v>0.54</v>
       </c>
       <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1702,17 +1696,17 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>07.10.2025 02:48</t>
+          <t>23.07.2025 10:51</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>8.241400000000001</v>
+        <v>0.3217</v>
       </c>
       <c r="G29" t="n">
         <v>100</v>
       </c>
       <c r="H29" t="n">
-        <v>824.14</v>
+        <v>32.17</v>
       </c>
       <c r="I29" t="n">
         <v>1</v>
@@ -1721,63 +1715,61 @@
         <v>0</v>
       </c>
       <c r="K29" t="n">
-        <v>5.82</v>
+        <v>1.57</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>03.09.2025 19:28</t>
+          <t>06.07.2025 18:12</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>2.3279</v>
+        <v>1.0717</v>
       </c>
       <c r="G30" t="n">
-        <v>100</v>
+        <v>87.38</v>
       </c>
       <c r="H30" t="n">
-        <v>232.79</v>
+        <v>93.65000000000001</v>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>1.6161</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
-        <v>3.56</v>
-      </c>
+        <v>0.57</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1787,85 +1779,83 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>03.07.2025 09:41</t>
+          <t>28.07.2025 08:54</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>2.7362</v>
+        <v>0.1686</v>
       </c>
       <c r="G31" t="n">
-        <v>143.96</v>
+        <v>58.12</v>
       </c>
       <c r="H31" t="n">
-        <v>393.9</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="I31" t="n">
-        <v>1</v>
+        <v>2.9247</v>
       </c>
       <c r="J31" t="n">
-        <v>0</v>
+        <v>-0.58</v>
       </c>
       <c r="K31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>05.10.2025 00:25</t>
+          <t>06.10.2025 19:41</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>8.6843</v>
+        <v>3.9832</v>
       </c>
       <c r="G32" t="n">
-        <v>100</v>
+        <v>103.2</v>
       </c>
       <c r="H32" t="n">
-        <v>868.4299999999999</v>
+        <v>411.07</v>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>2.0132</v>
       </c>
       <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
-        <v>7.54</v>
-      </c>
+        <v>-7.09</v>
+      </c>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1875,28 +1865,28 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>26.08.2025 18:55</t>
+          <t>02.10.2025 14:43</t>
         </is>
       </c>
       <c r="F33" t="n">
-        <v>0.6261</v>
+        <v>2.9602</v>
       </c>
       <c r="G33" t="n">
-        <v>113.85</v>
+        <v>187.89</v>
       </c>
       <c r="H33" t="n">
-        <v>71.28</v>
+        <v>556.1900000000001</v>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>2.2909</v>
       </c>
       <c r="J33" t="n">
-        <v>0</v>
+        <v>1.66</v>
       </c>
       <c r="K33" t="inlineStr"/>
     </row>
@@ -1923,17 +1913,17 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>02.07.2025 04:36</t>
+          <t>22.09.2025 13:11</t>
         </is>
       </c>
       <c r="F34" t="n">
-        <v>1.4676</v>
+        <v>8.353300000000001</v>
       </c>
       <c r="G34" t="n">
         <v>100</v>
       </c>
       <c r="H34" t="n">
-        <v>146.76</v>
+        <v>835.33</v>
       </c>
       <c r="I34" t="n">
         <v>1</v>
@@ -1942,23 +1932,23 @@
         <v>0</v>
       </c>
       <c r="K34" t="n">
-        <v>2.4</v>
+        <v>4.72</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1968,17 +1958,17 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09.10.2025 15:22</t>
+          <t>20.08.2025 19:30</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>8.102399999999999</v>
+        <v>1.1421</v>
       </c>
       <c r="G35" t="n">
-        <v>100</v>
+        <v>126.68</v>
       </c>
       <c r="H35" t="n">
-        <v>810.24</v>
+        <v>144.68</v>
       </c>
       <c r="I35" t="n">
         <v>1</v>
@@ -1986,24 +1976,22 @@
       <c r="J35" t="n">
         <v>0</v>
       </c>
-      <c r="K35" t="n">
-        <v>7.57</v>
-      </c>
+      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -2013,17 +2001,17 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>16.10.2025 18:31</t>
+          <t>12.09.2025 21:58</t>
         </is>
       </c>
       <c r="F36" t="n">
-        <v>6.3331</v>
+        <v>5.5961</v>
       </c>
       <c r="G36" t="n">
-        <v>147.1</v>
+        <v>105.59</v>
       </c>
       <c r="H36" t="n">
-        <v>931.6</v>
+        <v>590.89</v>
       </c>
       <c r="I36" t="n">
         <v>1</v>
@@ -2036,17 +2024,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2056,17 +2044,17 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>25.10.2025 07:28</t>
+          <t>08.08.2025 12:47</t>
         </is>
       </c>
       <c r="F37" t="n">
-        <v>6.682</v>
+        <v>2.2435</v>
       </c>
       <c r="G37" t="n">
-        <v>84.18000000000001</v>
+        <v>100</v>
       </c>
       <c r="H37" t="n">
-        <v>562.49</v>
+        <v>224.35</v>
       </c>
       <c r="I37" t="n">
         <v>1</v>
@@ -2074,55 +2062,59 @@
       <c r="J37" t="n">
         <v>0</v>
       </c>
-      <c r="K37" t="inlineStr"/>
+      <c r="K37" t="n">
+        <v>1.97</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>18.10.2025 06:48</t>
+          <t>13.08.2025 19:27</t>
         </is>
       </c>
       <c r="F38" t="n">
-        <v>6.1253</v>
+        <v>5.1647</v>
       </c>
       <c r="G38" t="n">
-        <v>152.58</v>
+        <v>100</v>
       </c>
       <c r="H38" t="n">
-        <v>934.6</v>
+        <v>516.47</v>
       </c>
       <c r="I38" t="n">
-        <v>1.7665</v>
+        <v>1</v>
       </c>
       <c r="J38" t="n">
-        <v>-4.21</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>8.19</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2142,17 +2134,17 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>11.09.2025 14:28</t>
+          <t>17.10.2025 10:49</t>
         </is>
       </c>
       <c r="F39" t="n">
-        <v>9.9201</v>
+        <v>9.859400000000001</v>
       </c>
       <c r="G39" t="n">
         <v>100</v>
       </c>
       <c r="H39" t="n">
-        <v>992.01</v>
+        <v>985.9400000000001</v>
       </c>
       <c r="I39" t="n">
         <v>1</v>
@@ -2161,66 +2153,68 @@
         <v>0</v>
       </c>
       <c r="K39" t="n">
-        <v>6.62</v>
+        <v>8.390000000000001</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>25.09.2025 08:28</t>
+          <t>27.08.2025 03:32</t>
         </is>
       </c>
       <c r="F40" t="n">
-        <v>3.8902</v>
+        <v>6.1098</v>
       </c>
       <c r="G40" t="n">
-        <v>166.53</v>
+        <v>100</v>
       </c>
       <c r="H40" t="n">
-        <v>647.84</v>
+        <v>610.98</v>
       </c>
       <c r="I40" t="n">
-        <v>3.6178</v>
+        <v>1</v>
       </c>
       <c r="J40" t="n">
-        <v>-2.77</v>
-      </c>
-      <c r="K40" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K40" t="n">
+        <v>1.49</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2230,17 +2224,17 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>15.09.2025 11:33</t>
+          <t>02.09.2025 13:16</t>
         </is>
       </c>
       <c r="F41" t="n">
-        <v>0.7306</v>
+        <v>2.6289</v>
       </c>
       <c r="G41" t="n">
-        <v>26.43</v>
+        <v>100</v>
       </c>
       <c r="H41" t="n">
-        <v>19.31</v>
+        <v>262.89</v>
       </c>
       <c r="I41" t="n">
         <v>1</v>
@@ -2248,22 +2242,24 @@
       <c r="J41" t="n">
         <v>0</v>
       </c>
-      <c r="K41" t="inlineStr"/>
+      <c r="K41" t="n">
+        <v>9.380000000000001</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2273,17 +2269,17 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>22.07.2025 03:50</t>
+          <t>13.07.2025 23:47</t>
         </is>
       </c>
       <c r="F42" t="n">
-        <v>4.6483</v>
+        <v>7.1079</v>
       </c>
       <c r="G42" t="n">
-        <v>187.03</v>
+        <v>122.94</v>
       </c>
       <c r="H42" t="n">
-        <v>869.37</v>
+        <v>873.85</v>
       </c>
       <c r="I42" t="n">
         <v>1</v>
@@ -2296,47 +2292,45 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>15.08.2025 06:33</t>
+          <t>22.10.2025 14:04</t>
         </is>
       </c>
       <c r="F43" t="n">
-        <v>5.5991</v>
+        <v>1.6256</v>
       </c>
       <c r="G43" t="n">
-        <v>100</v>
+        <v>61.43</v>
       </c>
       <c r="H43" t="n">
-        <v>559.91</v>
+        <v>99.86</v>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>1.4491</v>
       </c>
       <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>1.32</v>
-      </c>
+        <v>-1.47</v>
+      </c>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2361,17 +2355,17 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>11.09.2025 01:19</t>
+          <t>13.10.2025 16:17</t>
         </is>
       </c>
       <c r="F44" t="n">
-        <v>4.6717</v>
+        <v>7.2659</v>
       </c>
       <c r="G44" t="n">
-        <v>150.99</v>
+        <v>37.9</v>
       </c>
       <c r="H44" t="n">
-        <v>705.38</v>
+        <v>275.38</v>
       </c>
       <c r="I44" t="n">
         <v>1</v>
@@ -2384,12 +2378,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2404,17 +2398,17 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>19.08.2025 07:33</t>
+          <t>22.07.2025 17:03</t>
         </is>
       </c>
       <c r="F45" t="n">
-        <v>-0.4206</v>
+        <v>4.6243</v>
       </c>
       <c r="G45" t="n">
         <v>100</v>
       </c>
       <c r="H45" t="n">
-        <v>-42.06</v>
+        <v>462.43</v>
       </c>
       <c r="I45" t="n">
         <v>1</v>
@@ -2423,68 +2417,66 @@
         <v>0</v>
       </c>
       <c r="K45" t="n">
-        <v>1.25</v>
+        <v>8.609999999999999</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>23.10.2025 13:25</t>
+          <t>21.08.2025 18:07</t>
         </is>
       </c>
       <c r="F46" t="n">
-        <v>9.9696</v>
+        <v>9.034599999999999</v>
       </c>
       <c r="G46" t="n">
-        <v>100</v>
+        <v>155.37</v>
       </c>
       <c r="H46" t="n">
-        <v>996.96</v>
+        <v>1403.71</v>
       </c>
       <c r="I46" t="n">
-        <v>1</v>
+        <v>2.0417</v>
       </c>
       <c r="J46" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" t="n">
-        <v>6.25</v>
-      </c>
+        <v>-7.97</v>
+      </c>
+      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2494,17 +2486,17 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>20.09.2025 14:47</t>
+          <t>28.10.2025 11:12</t>
         </is>
       </c>
       <c r="F47" t="n">
-        <v>8.010199999999999</v>
+        <v>1.6173</v>
       </c>
       <c r="G47" t="n">
-        <v>100</v>
+        <v>45.65</v>
       </c>
       <c r="H47" t="n">
-        <v>801.02</v>
+        <v>73.83</v>
       </c>
       <c r="I47" t="n">
         <v>1</v>
@@ -2512,24 +2504,22 @@
       <c r="J47" t="n">
         <v>0</v>
       </c>
-      <c r="K47" t="n">
-        <v>5.02</v>
-      </c>
+      <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2539,17 +2529,17 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>11.07.2025 14:43</t>
+          <t>04.08.2025 04:52</t>
         </is>
       </c>
       <c r="F48" t="n">
-        <v>6.6415</v>
+        <v>3.7191</v>
       </c>
       <c r="G48" t="n">
-        <v>115.05</v>
+        <v>138.64</v>
       </c>
       <c r="H48" t="n">
-        <v>764.1</v>
+        <v>515.62</v>
       </c>
       <c r="I48" t="n">
         <v>1</v>
@@ -2562,107 +2552,103 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>23.08.2025 17:13</t>
+          <t>05.10.2025 11:56</t>
         </is>
       </c>
       <c r="F49" t="n">
-        <v>7.8097</v>
+        <v>8.8667</v>
       </c>
       <c r="G49" t="n">
-        <v>100</v>
+        <v>42.59</v>
       </c>
       <c r="H49" t="n">
-        <v>780.97</v>
+        <v>377.63</v>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>3.0099</v>
       </c>
       <c r="J49" t="n">
-        <v>0</v>
-      </c>
-      <c r="K49" t="n">
-        <v>4.34</v>
-      </c>
+        <v>-0.4</v>
+      </c>
+      <c r="K49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>14.07.2025 18:57</t>
+          <t>01.10.2025 09:21</t>
         </is>
       </c>
       <c r="F50" t="n">
-        <v>3.8787</v>
+        <v>0.9263</v>
       </c>
       <c r="G50" t="n">
-        <v>100</v>
+        <v>84.03</v>
       </c>
       <c r="H50" t="n">
-        <v>387.87</v>
+        <v>77.84</v>
       </c>
       <c r="I50" t="n">
-        <v>1</v>
+        <v>3.9813</v>
       </c>
       <c r="J50" t="n">
-        <v>0</v>
-      </c>
-      <c r="K50" t="n">
-        <v>6.18</v>
-      </c>
+        <v>-0.82</v>
+      </c>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2672,17 +2658,17 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>30.08.2025 07:17</t>
+          <t>06.07.2025 22:12</t>
         </is>
       </c>
       <c r="F51" t="n">
-        <v>4.7981</v>
+        <v>6.3093</v>
       </c>
       <c r="G51" t="n">
-        <v>124.92</v>
+        <v>100</v>
       </c>
       <c r="H51" t="n">
-        <v>599.38</v>
+        <v>630.9299999999999</v>
       </c>
       <c r="I51" t="n">
         <v>1</v>
@@ -2690,22 +2676,24 @@
       <c r="J51" t="n">
         <v>0</v>
       </c>
-      <c r="K51" t="inlineStr"/>
+      <c r="K51" t="n">
+        <v>8.27</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2715,17 +2703,17 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>30.09.2025 06:16</t>
+          <t>28.09.2025 20:50</t>
         </is>
       </c>
       <c r="F52" t="n">
-        <v>0.5106000000000001</v>
+        <v>7.9098</v>
       </c>
       <c r="G52" t="n">
-        <v>100</v>
+        <v>187.35</v>
       </c>
       <c r="H52" t="n">
-        <v>51.06</v>
+        <v>1481.9</v>
       </c>
       <c r="I52" t="n">
         <v>1</v>
@@ -2733,24 +2721,22 @@
       <c r="J52" t="n">
         <v>0</v>
       </c>
-      <c r="K52" t="n">
-        <v>8.279999999999999</v>
-      </c>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2760,17 +2746,17 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>06.07.2025 15:37</t>
+          <t>12.09.2025 05:41</t>
         </is>
       </c>
       <c r="F53" t="n">
-        <v>9.2286</v>
+        <v>2.8527</v>
       </c>
       <c r="G53" t="n">
-        <v>192.46</v>
+        <v>182.64</v>
       </c>
       <c r="H53" t="n">
-        <v>1776.14</v>
+        <v>521.02</v>
       </c>
       <c r="I53" t="n">
         <v>1</v>
@@ -2783,100 +2769,98 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>08.10.2025 02:30</t>
+          <t>02.09.2025 09:44</t>
         </is>
       </c>
       <c r="F54" t="n">
-        <v>7.2506</v>
+        <v>0.1616</v>
       </c>
       <c r="G54" t="n">
-        <v>100</v>
+        <v>135.92</v>
       </c>
       <c r="H54" t="n">
-        <v>725.0599999999999</v>
+        <v>21.96</v>
       </c>
       <c r="I54" t="n">
-        <v>1</v>
+        <v>1.2734</v>
       </c>
       <c r="J54" t="n">
-        <v>0</v>
-      </c>
-      <c r="K54" t="n">
-        <v>5.62</v>
-      </c>
+        <v>-9.199999999999999</v>
+      </c>
+      <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>18.10.2025 10:45</t>
+          <t>29.09.2025 10:10</t>
         </is>
       </c>
       <c r="F55" t="n">
-        <v>1.7387</v>
+        <v>6.4799</v>
       </c>
       <c r="G55" t="n">
-        <v>95.06</v>
+        <v>197.27</v>
       </c>
       <c r="H55" t="n">
-        <v>165.28</v>
+        <v>1278.29</v>
       </c>
       <c r="I55" t="n">
-        <v>1</v>
+        <v>2.204</v>
       </c>
       <c r="J55" t="n">
-        <v>0</v>
+        <v>-3.38</v>
       </c>
       <c r="K55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2886,45 +2870,45 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>15.09.2025 19:19</t>
+          <t>12.10.2025 04:40</t>
         </is>
       </c>
       <c r="F56" t="n">
-        <v>-0.1206</v>
+        <v>8.5936</v>
       </c>
       <c r="G56" t="n">
-        <v>194.66</v>
+        <v>108.09</v>
       </c>
       <c r="H56" t="n">
-        <v>-23.48</v>
+        <v>928.88</v>
       </c>
       <c r="I56" t="n">
-        <v>1</v>
+        <v>3.9688</v>
       </c>
       <c r="J56" t="n">
-        <v>0</v>
+        <v>-1.21</v>
       </c>
       <c r="K56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2934,17 +2918,17 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>16.09.2025 01:32</t>
+          <t>19.08.2025 01:16</t>
         </is>
       </c>
       <c r="F57" t="n">
-        <v>3.7047</v>
+        <v>7.7654</v>
       </c>
       <c r="G57" t="n">
-        <v>100</v>
+        <v>192.21</v>
       </c>
       <c r="H57" t="n">
-        <v>370.47</v>
+        <v>1492.59</v>
       </c>
       <c r="I57" t="n">
         <v>1</v>
@@ -2952,19 +2936,17 @@
       <c r="J57" t="n">
         <v>0</v>
       </c>
-      <c r="K57" t="n">
-        <v>1.19</v>
-      </c>
+      <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2974,71 +2956,71 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>17.10.2025 06:01</t>
+          <t>25.10.2025 18:26</t>
         </is>
       </c>
       <c r="F58" t="n">
-        <v>5.0838</v>
+        <v>5.8015</v>
       </c>
       <c r="G58" t="n">
-        <v>93.04000000000001</v>
+        <v>52.09</v>
       </c>
       <c r="H58" t="n">
-        <v>473</v>
+        <v>302.2</v>
       </c>
       <c r="I58" t="n">
-        <v>1.448</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>-6.98</v>
+        <v>0</v>
       </c>
       <c r="K58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>16.10.2025 00:18</t>
+          <t>12.09.2025 06:21</t>
         </is>
       </c>
       <c r="F59" t="n">
-        <v>0.188</v>
+        <v>0.7211</v>
       </c>
       <c r="G59" t="n">
-        <v>117.87</v>
+        <v>63.33</v>
       </c>
       <c r="H59" t="n">
-        <v>22.16</v>
+        <v>45.67</v>
       </c>
       <c r="I59" t="n">
-        <v>1.2333</v>
+        <v>1</v>
       </c>
       <c r="J59" t="n">
-        <v>-0.13</v>
+        <v>0</v>
       </c>
       <c r="K59" t="inlineStr"/>
     </row>
@@ -3065,17 +3047,17 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>01.09.2025 22:35</t>
+          <t>23.07.2025 15:24</t>
         </is>
       </c>
       <c r="F60" t="n">
-        <v>1.3818</v>
+        <v>5.1206</v>
       </c>
       <c r="G60" t="n">
         <v>100</v>
       </c>
       <c r="H60" t="n">
-        <v>138.18</v>
+        <v>512.0599999999999</v>
       </c>
       <c r="I60" t="n">
         <v>1</v>
@@ -3084,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="n">
-        <v>8.56</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="61">
@@ -3110,17 +3092,17 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>27.07.2025 11:00</t>
+          <t>20.10.2025 21:39</t>
         </is>
       </c>
       <c r="F61" t="n">
-        <v>0.6197</v>
+        <v>0.8633</v>
       </c>
       <c r="G61" t="n">
-        <v>44.47</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="H61" t="n">
-        <v>27.56</v>
+        <v>57.5</v>
       </c>
       <c r="I61" t="n">
         <v>1</v>
@@ -3133,60 +3115,60 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>06.10.2025 01:38</t>
+          <t>08.10.2025 03:18</t>
         </is>
       </c>
       <c r="F62" t="n">
-        <v>2.8286</v>
+        <v>7.9823</v>
       </c>
       <c r="G62" t="n">
-        <v>101.04</v>
+        <v>93.59999999999999</v>
       </c>
       <c r="H62" t="n">
-        <v>285.8</v>
+        <v>747.14</v>
       </c>
       <c r="I62" t="n">
-        <v>3.8485</v>
+        <v>1</v>
       </c>
       <c r="J62" t="n">
-        <v>-5.1</v>
+        <v>0</v>
       </c>
       <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -3196,17 +3178,17 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>25.07.2025 05:04</t>
+          <t>25.10.2025 06:46</t>
         </is>
       </c>
       <c r="F63" t="n">
-        <v>7.1012</v>
+        <v>5.3029</v>
       </c>
       <c r="G63" t="n">
-        <v>10.32</v>
+        <v>100</v>
       </c>
       <c r="H63" t="n">
-        <v>73.28</v>
+        <v>530.29</v>
       </c>
       <c r="I63" t="n">
         <v>1</v>
@@ -3214,7 +3196,9 @@
       <c r="J63" t="n">
         <v>0</v>
       </c>
-      <c r="K63" t="inlineStr"/>
+      <c r="K63" t="n">
+        <v>3.15</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3239,17 +3223,17 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>20.08.2025 14:51</t>
+          <t>06.07.2025 10:37</t>
         </is>
       </c>
       <c r="F64" t="n">
-        <v>1.5177</v>
+        <v>4.7092</v>
       </c>
       <c r="G64" t="n">
         <v>100</v>
       </c>
       <c r="H64" t="n">
-        <v>151.77</v>
+        <v>470.92</v>
       </c>
       <c r="I64" t="n">
         <v>1</v>
@@ -3258,23 +3242,23 @@
         <v>0</v>
       </c>
       <c r="K64" t="n">
-        <v>8.06</v>
+        <v>7.68</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3284,17 +3268,17 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>17.10.2025 00:37</t>
+          <t>05.08.2025 19:21</t>
         </is>
       </c>
       <c r="F65" t="n">
-        <v>-0.2623</v>
+        <v>3.5175</v>
       </c>
       <c r="G65" t="n">
-        <v>76.72</v>
+        <v>12.92</v>
       </c>
       <c r="H65" t="n">
-        <v>-20.12</v>
+        <v>45.45</v>
       </c>
       <c r="I65" t="n">
         <v>1</v>
@@ -3327,17 +3311,17 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>12.09.2025 18:29</t>
+          <t>18.09.2025 08:25</t>
         </is>
       </c>
       <c r="F66" t="n">
-        <v>2.3388</v>
+        <v>8.764900000000001</v>
       </c>
       <c r="G66" t="n">
         <v>100</v>
       </c>
       <c r="H66" t="n">
-        <v>233.88</v>
+        <v>876.49</v>
       </c>
       <c r="I66" t="n">
         <v>1</v>
@@ -3346,23 +3330,23 @@
         <v>0</v>
       </c>
       <c r="K66" t="n">
-        <v>5.71</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -3372,17 +3356,17 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>01.08.2025 15:06</t>
+          <t>21.07.2025 01:50</t>
         </is>
       </c>
       <c r="F67" t="n">
-        <v>9.5181</v>
+        <v>5.3896</v>
       </c>
       <c r="G67" t="n">
-        <v>18.18</v>
+        <v>100</v>
       </c>
       <c r="H67" t="n">
-        <v>173.04</v>
+        <v>538.96</v>
       </c>
       <c r="I67" t="n">
         <v>1</v>
@@ -3390,67 +3374,67 @@
       <c r="J67" t="n">
         <v>0</v>
       </c>
-      <c r="K67" t="inlineStr"/>
+      <c r="K67" t="n">
+        <v>0.71</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>04.10.2025 22:22</t>
+          <t>26.07.2025 23:15</t>
         </is>
       </c>
       <c r="F68" t="n">
-        <v>6.4845</v>
+        <v>6.3912</v>
       </c>
       <c r="G68" t="n">
-        <v>100</v>
+        <v>13.12</v>
       </c>
       <c r="H68" t="n">
-        <v>648.45</v>
+        <v>83.84999999999999</v>
       </c>
       <c r="I68" t="n">
-        <v>1</v>
+        <v>3.5793</v>
       </c>
       <c r="J68" t="n">
-        <v>0</v>
-      </c>
-      <c r="K68" t="n">
-        <v>9.91</v>
-      </c>
+        <v>-9.56</v>
+      </c>
+      <c r="K68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3460,17 +3444,17 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>04.09.2025 09:07</t>
+          <t>02.07.2025 13:56</t>
         </is>
       </c>
       <c r="F69" t="n">
-        <v>1.2176</v>
+        <v>1.289</v>
       </c>
       <c r="G69" t="n">
-        <v>100</v>
+        <v>76.23</v>
       </c>
       <c r="H69" t="n">
-        <v>121.76</v>
+        <v>98.26000000000001</v>
       </c>
       <c r="I69" t="n">
         <v>1</v>
@@ -3478,62 +3462,62 @@
       <c r="J69" t="n">
         <v>0</v>
       </c>
-      <c r="K69" t="n">
-        <v>2.07</v>
-      </c>
+      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>21.08.2025 16:57</t>
+          <t>10.10.2025 02:39</t>
         </is>
       </c>
       <c r="F70" t="n">
-        <v>9.8628</v>
+        <v>0.7994</v>
       </c>
       <c r="G70" t="n">
-        <v>47.9</v>
+        <v>100</v>
       </c>
       <c r="H70" t="n">
-        <v>472.43</v>
+        <v>79.94</v>
       </c>
       <c r="I70" t="n">
-        <v>2.1046</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>-9.91</v>
-      </c>
-      <c r="K70" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.99</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -3548,17 +3532,17 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>19.08.2025 10:46</t>
+          <t>02.09.2025 15:37</t>
         </is>
       </c>
       <c r="F71" t="n">
-        <v>4.8413</v>
+        <v>6.571</v>
       </c>
       <c r="G71" t="n">
         <v>100</v>
       </c>
       <c r="H71" t="n">
-        <v>484.13</v>
+        <v>657.1</v>
       </c>
       <c r="I71" t="n">
         <v>1</v>
@@ -3567,23 +3551,23 @@
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>9.84</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3593,17 +3577,17 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>15.07.2025 18:08</t>
+          <t>01.09.2025 19:36</t>
         </is>
       </c>
       <c r="F72" t="n">
-        <v>3.6566</v>
+        <v>0.075</v>
       </c>
       <c r="G72" t="n">
-        <v>100</v>
+        <v>169.94</v>
       </c>
       <c r="H72" t="n">
-        <v>365.66</v>
+        <v>12.75</v>
       </c>
       <c r="I72" t="n">
         <v>1</v>
@@ -3611,19 +3595,17 @@
       <c r="J72" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="n">
-        <v>8.800000000000001</v>
-      </c>
+      <c r="K72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -3633,45 +3615,45 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>20.07.2025 18:01</t>
+          <t>26.07.2025 19:39</t>
         </is>
       </c>
       <c r="F73" t="n">
-        <v>2.042</v>
+        <v>3.9384</v>
       </c>
       <c r="G73" t="n">
-        <v>109.84</v>
+        <v>108.06</v>
       </c>
       <c r="H73" t="n">
-        <v>224.29</v>
+        <v>425.58</v>
       </c>
       <c r="I73" t="n">
-        <v>3.6325</v>
+        <v>1</v>
       </c>
       <c r="J73" t="n">
-        <v>-7.43</v>
+        <v>0</v>
       </c>
       <c r="K73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3681,17 +3663,17 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>20.10.2025 22:11</t>
+          <t>05.09.2025 14:44</t>
         </is>
       </c>
       <c r="F74" t="n">
-        <v>6.0498</v>
+        <v>-0.1898</v>
       </c>
       <c r="G74" t="n">
-        <v>100</v>
+        <v>168.24</v>
       </c>
       <c r="H74" t="n">
-        <v>604.98</v>
+        <v>-31.93</v>
       </c>
       <c r="I74" t="n">
         <v>1</v>
@@ -3699,105 +3681,103 @@
       <c r="J74" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="n">
-        <v>0.9</v>
-      </c>
+      <c r="K74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>02.10.2025 10:47</t>
+          <t>08.08.2025 11:53</t>
         </is>
       </c>
       <c r="F75" t="n">
-        <v>6.0494</v>
+        <v>0.4552</v>
       </c>
       <c r="G75" t="n">
-        <v>47.6</v>
+        <v>124.86</v>
       </c>
       <c r="H75" t="n">
-        <v>287.95</v>
+        <v>56.84</v>
       </c>
       <c r="I75" t="n">
-        <v>2.0614</v>
+        <v>1</v>
       </c>
       <c r="J75" t="n">
-        <v>1.07</v>
+        <v>0</v>
       </c>
       <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>27.08.2025 12:39</t>
+          <t>04.07.2025 13:00</t>
         </is>
       </c>
       <c r="F76" t="n">
-        <v>6.0259</v>
+        <v>5.9142</v>
       </c>
       <c r="G76" t="n">
-        <v>111.93</v>
+        <v>16.58</v>
       </c>
       <c r="H76" t="n">
-        <v>674.48</v>
+        <v>98.06</v>
       </c>
       <c r="I76" t="n">
-        <v>1</v>
+        <v>1.0935</v>
       </c>
       <c r="J76" t="n">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -3812,17 +3792,17 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>26.09.2025 04:20</t>
+          <t>01.10.2025 02:25</t>
         </is>
       </c>
       <c r="F77" t="n">
-        <v>-0.0527</v>
+        <v>7.71</v>
       </c>
       <c r="G77" t="n">
         <v>100</v>
       </c>
       <c r="H77" t="n">
-        <v>-5.27</v>
+        <v>771</v>
       </c>
       <c r="I77" t="n">
         <v>1</v>
@@ -3831,13 +3811,13 @@
         <v>0</v>
       </c>
       <c r="K77" t="n">
-        <v>7.89</v>
+        <v>5.05</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3857,17 +3837,17 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>16.10.2025 11:29</t>
+          <t>22.07.2025 02:58</t>
         </is>
       </c>
       <c r="F78" t="n">
-        <v>7.8581</v>
+        <v>9.067600000000001</v>
       </c>
       <c r="G78" t="n">
         <v>100</v>
       </c>
       <c r="H78" t="n">
-        <v>785.8099999999999</v>
+        <v>906.76</v>
       </c>
       <c r="I78" t="n">
         <v>1</v>
@@ -3876,23 +3856,23 @@
         <v>0</v>
       </c>
       <c r="K78" t="n">
-        <v>4.93</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3902,17 +3882,17 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>23.08.2025 19:45</t>
+          <t>13.07.2025 22:36</t>
         </is>
       </c>
       <c r="F79" t="n">
-        <v>4.0955</v>
+        <v>4.6013</v>
       </c>
       <c r="G79" t="n">
-        <v>176.02</v>
+        <v>100</v>
       </c>
       <c r="H79" t="n">
-        <v>720.89</v>
+        <v>460.13</v>
       </c>
       <c r="I79" t="n">
         <v>1</v>
@@ -3920,22 +3900,24 @@
       <c r="J79" t="n">
         <v>0</v>
       </c>
-      <c r="K79" t="inlineStr"/>
+      <c r="K79" t="n">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -3945,17 +3927,17 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>19.07.2025 17:50</t>
+          <t>03.10.2025 06:22</t>
         </is>
       </c>
       <c r="F80" t="n">
-        <v>7.1635</v>
+        <v>5.1373</v>
       </c>
       <c r="G80" t="n">
-        <v>195.77</v>
+        <v>100</v>
       </c>
       <c r="H80" t="n">
-        <v>1402.4</v>
+        <v>513.73</v>
       </c>
       <c r="I80" t="n">
         <v>1</v>
@@ -3963,52 +3945,52 @@
       <c r="J80" t="n">
         <v>0</v>
       </c>
-      <c r="K80" t="inlineStr"/>
+      <c r="K80" t="n">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>08.07.2025 10:17</t>
+          <t>05.09.2025 14:14</t>
         </is>
       </c>
       <c r="F81" t="n">
-        <v>8.763</v>
+        <v>1.723</v>
       </c>
       <c r="G81" t="n">
-        <v>100</v>
+        <v>57.58</v>
       </c>
       <c r="H81" t="n">
-        <v>876.3</v>
+        <v>99.20999999999999</v>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>3.9062</v>
       </c>
       <c r="J81" t="n">
-        <v>0</v>
-      </c>
-      <c r="K81" t="n">
-        <v>1.87</v>
-      </c>
+        <v>-7.96</v>
+      </c>
+      <c r="K81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4033,17 +4015,17 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>17.09.2025 09:39</t>
+          <t>11.08.2025 01:37</t>
         </is>
       </c>
       <c r="F82" t="n">
-        <v>7.5972</v>
+        <v>5.7187</v>
       </c>
       <c r="G82" t="n">
         <v>100</v>
       </c>
       <c r="H82" t="n">
-        <v>759.72</v>
+        <v>571.87</v>
       </c>
       <c r="I82" t="n">
         <v>1</v>
@@ -4052,23 +4034,23 @@
         <v>0</v>
       </c>
       <c r="K82" t="n">
-        <v>2.41</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -4078,17 +4060,17 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>13.08.2025 05:50</t>
+          <t>21.08.2025 23:08</t>
         </is>
       </c>
       <c r="F83" t="n">
-        <v>7.5718</v>
+        <v>5.0375</v>
       </c>
       <c r="G83" t="n">
-        <v>141.73</v>
+        <v>100</v>
       </c>
       <c r="H83" t="n">
-        <v>1073.15</v>
+        <v>503.75</v>
       </c>
       <c r="I83" t="n">
         <v>1</v>
@@ -4096,17 +4078,19 @@
       <c r="J83" t="n">
         <v>0</v>
       </c>
-      <c r="K83" t="inlineStr"/>
+      <c r="K83" t="n">
+        <v>5.03</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10-year EDO bonds</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -4121,17 +4105,17 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>02.09.2025 06:38</t>
+          <t>18.08.2025 04:43</t>
         </is>
       </c>
       <c r="F84" t="n">
-        <v>6.8628</v>
+        <v>2.0454</v>
       </c>
       <c r="G84" t="n">
         <v>100</v>
       </c>
       <c r="H84" t="n">
-        <v>686.28</v>
+        <v>204.54</v>
       </c>
       <c r="I84" t="n">
         <v>1</v>
@@ -4140,18 +4124,18 @@
         <v>0</v>
       </c>
       <c r="K84" t="n">
-        <v>5.84</v>
+        <v>7.77</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>US0378331005</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>Apple Inc</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -4161,35 +4145,35 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>02.07.2025 00:45</t>
+          <t>19.10.2025 16:36</t>
         </is>
       </c>
       <c r="F85" t="n">
-        <v>0.8605</v>
+        <v>1.2291</v>
       </c>
       <c r="G85" t="n">
-        <v>13.68</v>
+        <v>199.39</v>
       </c>
       <c r="H85" t="n">
-        <v>11.77</v>
+        <v>245.07</v>
       </c>
       <c r="I85" t="n">
-        <v>1</v>
+        <v>3.0258</v>
       </c>
       <c r="J85" t="n">
-        <v>0</v>
+        <v>-0.73</v>
       </c>
       <c r="K85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4209,17 +4193,17 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>26.10.2025 13:31</t>
+          <t>03.08.2025 20:30</t>
         </is>
       </c>
       <c r="F86" t="n">
-        <v>8.828200000000001</v>
+        <v>4.5474</v>
       </c>
       <c r="G86" t="n">
         <v>100</v>
       </c>
       <c r="H86" t="n">
-        <v>882.8200000000001</v>
+        <v>454.74</v>
       </c>
       <c r="I86" t="n">
         <v>1</v>
@@ -4228,18 +4212,18 @@
         <v>0</v>
       </c>
       <c r="K86" t="n">
-        <v>1.26</v>
+        <v>9.039999999999999</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -4249,28 +4233,28 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>20.10.2025 00:57</t>
+          <t>07.07.2025 06:37</t>
         </is>
       </c>
       <c r="F87" t="n">
-        <v>1.2942</v>
+        <v>-0.4171</v>
       </c>
       <c r="G87" t="n">
-        <v>21.89</v>
+        <v>169.9</v>
       </c>
       <c r="H87" t="n">
-        <v>28.33</v>
+        <v>-70.87</v>
       </c>
       <c r="I87" t="n">
-        <v>1</v>
+        <v>1.7345</v>
       </c>
       <c r="J87" t="n">
-        <v>0</v>
+        <v>-1.82</v>
       </c>
       <c r="K87" t="inlineStr"/>
     </row>
@@ -4297,17 +4281,17 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>13.07.2025 13:29</t>
+          <t>07.08.2025 17:06</t>
         </is>
       </c>
       <c r="F88" t="n">
-        <v>4.743</v>
+        <v>6.5902</v>
       </c>
       <c r="G88" t="n">
         <v>100</v>
       </c>
       <c r="H88" t="n">
-        <v>474.3</v>
+        <v>659.02</v>
       </c>
       <c r="I88" t="n">
         <v>1</v>
@@ -4316,23 +4300,23 @@
         <v>0</v>
       </c>
       <c r="K88" t="n">
-        <v>6.77</v>
+        <v>9.56</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>PLBETF400025</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>mWIG40TR Beta ETF</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>ETF</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -4342,17 +4326,17 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>05.08.2025 22:43</t>
+          <t>10.08.2025 22:49</t>
         </is>
       </c>
       <c r="F89" t="n">
-        <v>2.7505</v>
+        <v>3.76</v>
       </c>
       <c r="G89" t="n">
-        <v>161.17</v>
+        <v>136.09</v>
       </c>
       <c r="H89" t="n">
-        <v>443.3</v>
+        <v>511.7</v>
       </c>
       <c r="I89" t="n">
         <v>1</v>
@@ -4365,17 +4349,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4385,17 +4369,17 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>24.10.2025 22:57</t>
+          <t>10.08.2025 01:43</t>
         </is>
       </c>
       <c r="F90" t="n">
-        <v>7.6309</v>
+        <v>0.4492</v>
       </c>
       <c r="G90" t="n">
-        <v>68.2</v>
+        <v>100</v>
       </c>
       <c r="H90" t="n">
-        <v>520.4299999999999</v>
+        <v>44.92</v>
       </c>
       <c r="I90" t="n">
         <v>1</v>
@@ -4403,17 +4387,19 @@
       <c r="J90" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr"/>
+      <c r="K90" t="n">
+        <v>8.08</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>IE00B6R52259</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>iShares MSCI ACWI UCITS ETF</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -4423,40 +4409,40 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>PLN</t>
+          <t>USD</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>17.08.2025 20:30</t>
+          <t>09.08.2025 22:20</t>
         </is>
       </c>
       <c r="F91" t="n">
-        <v>2.0673</v>
+        <v>7.7739</v>
       </c>
       <c r="G91" t="n">
-        <v>192.09</v>
+        <v>198.76</v>
       </c>
       <c r="H91" t="n">
-        <v>397.11</v>
+        <v>1545.14</v>
       </c>
       <c r="I91" t="n">
-        <v>1</v>
+        <v>3.0486</v>
       </c>
       <c r="J91" t="n">
-        <v>0</v>
+        <v>1.55</v>
       </c>
       <c r="K91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -4471,17 +4457,17 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>07.07.2025 21:12</t>
+          <t>14.08.2025 17:48</t>
         </is>
       </c>
       <c r="F92" t="n">
-        <v>7.2461</v>
+        <v>2.562</v>
       </c>
       <c r="G92" t="n">
         <v>100</v>
       </c>
       <c r="H92" t="n">
-        <v>724.61</v>
+        <v>256.2</v>
       </c>
       <c r="I92" t="n">
         <v>1</v>
@@ -4490,23 +4476,23 @@
         <v>0</v>
       </c>
       <c r="K92" t="n">
-        <v>6.84</v>
+        <v>1.49</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>PLBLOCM00013</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Cannabis Poland</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>SHARE</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -4516,17 +4502,17 @@
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>07.07.2025 17:21</t>
+          <t>21.10.2025 22:32</t>
         </is>
       </c>
       <c r="F93" t="n">
-        <v>3.6025</v>
+        <v>8.9811</v>
       </c>
       <c r="G93" t="n">
-        <v>73.36</v>
+        <v>100</v>
       </c>
       <c r="H93" t="n">
-        <v>264.28</v>
+        <v>898.11</v>
       </c>
       <c r="I93" t="n">
         <v>1</v>
@@ -4534,55 +4520,59 @@
       <c r="J93" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr"/>
+      <c r="K93" t="n">
+        <v>3.35</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>07.09.2025 04:42</t>
+          <t>27.07.2025 09:24</t>
         </is>
       </c>
       <c r="F94" t="n">
-        <v>1.1397</v>
+        <v>7.953</v>
       </c>
       <c r="G94" t="n">
-        <v>150.22</v>
+        <v>100</v>
       </c>
       <c r="H94" t="n">
-        <v>171.21</v>
+        <v>795.3</v>
       </c>
       <c r="I94" t="n">
-        <v>3.2723</v>
+        <v>1</v>
       </c>
       <c r="J94" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="K94" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K94" t="n">
+        <v>7.79</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>EDO0935</t>
+          <t>EDO1035</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -4602,17 +4592,17 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>09.08.2025 00:33</t>
+          <t>29.08.2025 21:36</t>
         </is>
       </c>
       <c r="F95" t="n">
-        <v>6.7151</v>
+        <v>1.1216</v>
       </c>
       <c r="G95" t="n">
         <v>100</v>
       </c>
       <c r="H95" t="n">
-        <v>671.51</v>
+        <v>112.16</v>
       </c>
       <c r="I95" t="n">
         <v>1</v>
@@ -4621,7 +4611,7 @@
         <v>0</v>
       </c>
       <c r="K95" t="n">
-        <v>2.45</v>
+        <v>5.12</v>
       </c>
     </row>
     <row r="96">
@@ -4647,17 +4637,17 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>11.10.2025 06:52</t>
+          <t>04.10.2025 07:10</t>
         </is>
       </c>
       <c r="F96" t="n">
-        <v>7.9939</v>
+        <v>3.3501</v>
       </c>
       <c r="G96" t="n">
         <v>100</v>
       </c>
       <c r="H96" t="n">
-        <v>799.39</v>
+        <v>335.01</v>
       </c>
       <c r="I96" t="n">
         <v>1</v>
@@ -4666,13 +4656,13 @@
         <v>0</v>
       </c>
       <c r="K96" t="n">
-        <v>8.640000000000001</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>EDO1035</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -4692,17 +4682,17 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>24.09.2025 03:18</t>
+          <t>29.08.2025 09:32</t>
         </is>
       </c>
       <c r="F97" t="n">
-        <v>7.0156</v>
+        <v>7.498</v>
       </c>
       <c r="G97" t="n">
         <v>100</v>
       </c>
       <c r="H97" t="n">
-        <v>701.5599999999999</v>
+        <v>749.8</v>
       </c>
       <c r="I97" t="n">
         <v>1</v>
@@ -4711,18 +4701,18 @@
         <v>0</v>
       </c>
       <c r="K97" t="n">
-        <v>1.6</v>
+        <v>6.14</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>EDO0935</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>10-year EDO bonds</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -4737,17 +4727,17 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>03.08.2025 17:19</t>
+          <t>09.10.2025 17:29</t>
         </is>
       </c>
       <c r="F98" t="n">
-        <v>0.419</v>
+        <v>5.4945</v>
       </c>
       <c r="G98" t="n">
         <v>100</v>
       </c>
       <c r="H98" t="n">
-        <v>41.9</v>
+        <v>549.45</v>
       </c>
       <c r="I98" t="n">
         <v>1</v>
@@ -4756,23 +4746,23 @@
         <v>0</v>
       </c>
       <c r="K98" t="n">
-        <v>2.75</v>
+        <v>8.449999999999999</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>COI0829</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>4-year COI bonds</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>BOND</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4782,17 +4772,17 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>22.08.2025 19:16</t>
+          <t>18.10.2025 01:15</t>
         </is>
       </c>
       <c r="F99" t="n">
-        <v>4.3654</v>
+        <v>9.0351</v>
       </c>
       <c r="G99" t="n">
-        <v>100</v>
+        <v>73.84999999999999</v>
       </c>
       <c r="H99" t="n">
-        <v>436.54</v>
+        <v>667.24</v>
       </c>
       <c r="I99" t="n">
         <v>1</v>
@@ -4800,67 +4790,67 @@
       <c r="J99" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="n">
-        <v>4.4</v>
-      </c>
+      <c r="K99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>IE00B6R52259</t>
+          <t>COI0829</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>iShares MSCI ACWI UCITS ETF</t>
+          <t>4-year COI bonds</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>BOND</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>USD</t>
+          <t>PLN</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>01.07.2025 14:55</t>
+          <t>21.10.2025 05:03</t>
         </is>
       </c>
       <c r="F100" t="n">
-        <v>7.6907</v>
+        <v>5.8814</v>
       </c>
       <c r="G100" t="n">
-        <v>41.63</v>
+        <v>100</v>
       </c>
       <c r="H100" t="n">
-        <v>320.16</v>
+        <v>588.14</v>
       </c>
       <c r="I100" t="n">
-        <v>1.591</v>
+        <v>1</v>
       </c>
       <c r="J100" t="n">
-        <v>-3.99</v>
-      </c>
-      <c r="K100" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K100" t="n">
+        <v>2.75</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>PLBETF400025</t>
+          <t>PLBLOCM00013</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>mWIG40TR Beta ETF</t>
+          <t>Cannabis Poland</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>ETF</t>
+          <t>SHARE</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4870,17 +4860,17 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>21.10.2025 13:25</t>
+          <t>16.08.2025 15:50</t>
         </is>
       </c>
       <c r="F101" t="n">
-        <v>-0.2165</v>
+        <v>5.4462</v>
       </c>
       <c r="G101" t="n">
-        <v>28.15</v>
+        <v>67.06999999999999</v>
       </c>
       <c r="H101" t="n">
-        <v>-6.09</v>
+        <v>365.28</v>
       </c>
       <c r="I101" t="n">
         <v>1</v>

</xml_diff>